<commit_message>
Updated DatePicker in cabBooking Page and few bugfixes
</commit_message>
<xml_diff>
--- a/src/test/resources/testData/test.xlsx
+++ b/src/test/resources/testData/test.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://cognizantonline-my.sharepoint.com/personal/2406654_cognizant_com/Documents/Documents/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\2407474\git\MakeMyTrip_FinalProject\src\test\resources\testData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="58" documentId="8_{7511C706-69B9-4D2A-A091-A05338DCF64B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{93CB8A10-AE8D-4CB8-90E1-6FFF12ACF839}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AB245527-17E7-4CA8-9EEA-68A7649296F2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{C58A9C54-FA6C-468B-AA20-BB7B0947786D}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" activeTab="1" xr2:uid="{C58A9C54-FA6C-468B-AA20-BB7B0947786D}"/>
   </bookViews>
   <sheets>
     <sheet name="CabBooking1" sheetId="1" r:id="rId1"/>
@@ -75,79 +75,79 @@
     <t>Kargil</t>
   </si>
   <si>
+    <t>Email</t>
+  </si>
+  <si>
+    <t>Sender Name</t>
+  </si>
+  <si>
+    <t>Mobile no.</t>
+  </si>
+  <si>
+    <t>Sahil</t>
+  </si>
+  <si>
+    <t>invalid-email</t>
+  </si>
+  <si>
+    <t>Recipient1</t>
+  </si>
+  <si>
+    <t>Recipient2</t>
+  </si>
+  <si>
+    <t>Abhinav</t>
+  </si>
+  <si>
+    <t>r1gmail.com</t>
+  </si>
+  <si>
+    <t>R2#gmail.com</t>
+  </si>
+  <si>
+    <t>abhinav@gm.com</t>
+  </si>
+  <si>
+    <t>Alice</t>
+  </si>
+  <si>
+    <t>234QWE122@GMAIL.COM</t>
+  </si>
+  <si>
+    <t>Happy Birthday!</t>
+  </si>
+  <si>
+    <t>Sender Name1</t>
+  </si>
+  <si>
+    <t>Mobile 1</t>
+  </si>
+  <si>
+    <t>Email 1</t>
+  </si>
+  <si>
+    <t>Sender Name2</t>
+  </si>
+  <si>
+    <t>Mobile 2</t>
+  </si>
+  <si>
+    <t>Email 2</t>
+  </si>
+  <si>
+    <t>Sender Name3</t>
+  </si>
+  <si>
+    <t>Mobile 3</t>
+  </si>
+  <si>
+    <t>Email 3</t>
+  </si>
+  <si>
+    <t>Message</t>
+  </si>
+  <si>
     <t>Jul 25 2025</t>
-  </si>
-  <si>
-    <t>Email</t>
-  </si>
-  <si>
-    <t>Sender Name</t>
-  </si>
-  <si>
-    <t>Mobile no.</t>
-  </si>
-  <si>
-    <t>Sahil</t>
-  </si>
-  <si>
-    <t>invalid-email</t>
-  </si>
-  <si>
-    <t>Recipient1</t>
-  </si>
-  <si>
-    <t>Recipient2</t>
-  </si>
-  <si>
-    <t>Abhinav</t>
-  </si>
-  <si>
-    <t>r1gmail.com</t>
-  </si>
-  <si>
-    <t>R2#gmail.com</t>
-  </si>
-  <si>
-    <t>abhinav@gm.com</t>
-  </si>
-  <si>
-    <t>Alice</t>
-  </si>
-  <si>
-    <t>234QWE122@GMAIL.COM</t>
-  </si>
-  <si>
-    <t>Happy Birthday!</t>
-  </si>
-  <si>
-    <t>Sender Name1</t>
-  </si>
-  <si>
-    <t>Mobile 1</t>
-  </si>
-  <si>
-    <t>Email 1</t>
-  </si>
-  <si>
-    <t>Sender Name2</t>
-  </si>
-  <si>
-    <t>Mobile 2</t>
-  </si>
-  <si>
-    <t>Email 2</t>
-  </si>
-  <si>
-    <t>Sender Name3</t>
-  </si>
-  <si>
-    <t>Mobile 3</t>
-  </si>
-  <si>
-    <t>Email 3</t>
-  </si>
-  <si>
-    <t>Message</t>
   </si>
 </sst>
 </file>
@@ -205,10 +205,6 @@
     </ext>
   </extLst>
 </styleSheet>
-</file>
-
-<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
-<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -530,7 +526,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{80605DAD-2886-48AA-A94E-420496177FDB}">
   <dimension ref="A1:E2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="D1" sqref="D1"/>
     </sheetView>
   </sheetViews>
@@ -586,8 +582,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0FBD98C3-9F02-4CF6-9A7E-F708DA8C0291}">
   <dimension ref="A1:D2"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C5" sqref="C5"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -620,7 +616,7 @@
         <v>10</v>
       </c>
       <c r="C2" t="s">
-        <v>11</v>
+        <v>35</v>
       </c>
       <c r="D2" s="2">
         <v>0.41666666666666669</v>
@@ -649,24 +645,24 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B1" t="s">
         <v>13</v>
       </c>
-      <c r="B1" t="s">
-        <v>14</v>
-      </c>
       <c r="C1" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B2">
         <v>9876543210</v>
       </c>
       <c r="C2" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
   </sheetData>
@@ -697,60 +693,60 @@
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
+        <v>25</v>
+      </c>
+      <c r="B1" t="s">
         <v>26</v>
       </c>
-      <c r="B1" t="s">
+      <c r="C1" t="s">
         <v>27</v>
       </c>
-      <c r="C1" t="s">
+      <c r="D1" t="s">
         <v>28</v>
       </c>
-      <c r="D1" t="s">
+      <c r="E1" t="s">
         <v>29</v>
       </c>
-      <c r="E1" t="s">
+      <c r="F1" t="s">
         <v>30</v>
       </c>
-      <c r="F1" t="s">
+      <c r="G1" t="s">
         <v>31</v>
       </c>
-      <c r="G1" t="s">
+      <c r="H1" t="s">
         <v>32</v>
       </c>
-      <c r="H1" t="s">
+      <c r="I1" t="s">
         <v>33</v>
-      </c>
-      <c r="I1" t="s">
-        <v>34</v>
       </c>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B2">
         <v>1234567890</v>
       </c>
       <c r="C2" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="D2" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="E2">
         <v>2345678901</v>
       </c>
       <c r="F2" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="G2" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="H2">
         <v>9502377742</v>
       </c>
       <c r="I2" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
     </row>
   </sheetData>
@@ -776,30 +772,30 @@
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B1" t="s">
         <v>13</v>
       </c>
-      <c r="B1" t="s">
-        <v>14</v>
-      </c>
       <c r="C1" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="D1" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B2">
         <v>4567891230</v>
       </c>
       <c r="C2" t="s">
+        <v>23</v>
+      </c>
+      <c r="D2" t="s">
         <v>24</v>
-      </c>
-      <c r="D2" t="s">
-        <v>25</v>
       </c>
     </row>
   </sheetData>

</xml_diff>